<commit_message>
Memperbaiki tanggal terakhir tes di forecast
</commit_message>
<xml_diff>
--- a/public/excel/import.xlsx
+++ b/public/excel/import.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\trn\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A2CECF-D635-4445-94DA-C7E895883038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$AI$10</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,13 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Data Perpanjangan License Expired Februari 2022</t>
-  </si>
-  <si>
-    <t>Tanggal 8 November 2021</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>NIK</t>
   </si>
@@ -38,9 +36,6 @@
     <t>Nama</t>
   </si>
   <si>
-    <t>Line/Unit Kerja</t>
-  </si>
-  <si>
     <t>Shift</t>
   </si>
   <si>
@@ -51,12 +46,33 @@
   </si>
   <si>
     <t>Bulan Expired</t>
+  </si>
+  <si>
+    <t>Carline</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Carcode</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Tanggal_tes</t>
+  </si>
+  <si>
+    <t>Bulan Expired :</t>
+  </si>
+  <si>
+    <t>Tes Terakhir :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,7 +96,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,11 +119,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -116,6 +141,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -397,81 +438,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AO4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5">
+        <v>44750</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="I4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="9"/>
+      <c r="AN4" s="9"/>
+      <c r="AO4" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G4:AE4"/>
+    <mergeCell ref="K4:AO4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>